<commit_message>
Wait, adding more to my two lines of data!
</commit_message>
<xml_diff>
--- a/analyses/scrapeUSDAseedmanual/scraping/usdaDataScraping_EMW.xlsx
+++ b/analyses/scrapeUSDAseedmanual/scraping/usdaDataScraping_EMW.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lizzie/Documents/git/projects/egret/analyses/scrapeUSDAseedmanual/scraping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6CE70FE-09C9-9A49-A123-2AD186B1D4A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1CDE7C-2229-944D-ABF5-876322FBD4F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2560" yWindow="1260" windowWidth="30180" windowHeight="22780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="63">
   <si>
     <t>pdf_page_number</t>
   </si>
@@ -237,6 +237,9 @@
   </si>
   <si>
     <t>dash</t>
+  </si>
+  <si>
+    <t>1 to 6</t>
   </si>
 </sst>
 </file>
@@ -279,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -290,6 +293,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -967,7 +971,10 @@
       <c r="F2" t="s">
         <v>58</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="L2" t="s">
         <v>60</v>
       </c>
       <c r="M2">
@@ -981,6 +988,9 @@
       </c>
       <c r="Q2">
         <v>30</v>
+      </c>
+      <c r="U2">
+        <v>70</v>
       </c>
       <c r="V2" t="s">
         <v>61</v>
@@ -1002,7 +1012,10 @@
       <c r="F3" t="s">
         <v>59</v>
       </c>
-      <c r="J3">
+      <c r="J3" t="s">
+        <v>62</v>
+      </c>
+      <c r="L3">
         <v>120</v>
       </c>
       <c r="M3">
@@ -1016,6 +1029,9 @@
       </c>
       <c r="Q3">
         <v>70</v>
+      </c>
+      <c r="U3">
+        <v>62</v>
       </c>
       <c r="V3">
         <v>50</v>

</xml_diff>

<commit_message>
Updated REAMDE for pointer to USDA and my USDA data entry
</commit_message>
<xml_diff>
--- a/analyses/scrapeUSDAseedmanual/scraping/usdaDataScraping_EMW.xlsx
+++ b/analyses/scrapeUSDAseedmanual/scraping/usdaDataScraping_EMW.xlsx
@@ -8,25 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lizzie/Documents/git/projects/egret/analyses/scrapeUSDAseedmanual/scraping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1CDE7C-2229-944D-ABF5-876322FBD4F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB27D429-5413-4C49-AC5D-39E1FD42A8FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="1260" windowWidth="30180" windowHeight="22780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22400" yWindow="500" windowWidth="24780" windowHeight="23620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Meta" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="129">
   <si>
     <t>pdf_page_number</t>
   </si>
@@ -142,10 +152,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>any pretreatment before the germination</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>temperature of stratification</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -185,18 +191,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>total germination percentage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>averaged germination percentage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>germination rate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>averaged germinative energy percentage</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -221,6 +215,65 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>50%_germ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>any pretreatment before the germination (chemical, storage)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>germination ratec (only the percentage data)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>total germination percentage (if it is germination percentage without any specification, data should go to this column)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>averaged germination percentage (only enter here if it specify it's average germination percentage)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Any information you think will be helpful for data cleaning later</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>days of 50% germination</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Extra notes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>All the ranges should be entered as 'to', e.g.: "5-10" in the table should be entered as "5 to 10"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If it is a dash in the table, it is NA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>For cold stratification and warm stratification, if they specify in the table it is 0, I think we should enter them as 0 instead of leaving them as blank</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>avg_germination_percent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>total_germination_percent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>germination_time_days</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Amelanchier</t>
   </si>
   <si>
@@ -230,23 +283,188 @@
     <t>sand</t>
   </si>
   <si>
+    <t>1 to 6</t>
+  </si>
+  <si>
     <t>sand or blotters</t>
   </si>
   <si>
     <t>180+</t>
   </si>
   <si>
-    <t>dash</t>
-  </si>
-  <si>
-    <t>1 to 6</t>
+    <t>alnifolia var. semiintegrifolia</t>
+  </si>
+  <si>
+    <t>kimpack</t>
+  </si>
+  <si>
+    <t>sand or sand and peat</t>
+  </si>
+  <si>
+    <t>filter paper</t>
+  </si>
+  <si>
+    <t>30 to 90</t>
+  </si>
+  <si>
+    <t>90 to 120</t>
+  </si>
+  <si>
+    <t>60+</t>
+  </si>
+  <si>
+    <t>6 to 7</t>
+  </si>
+  <si>
+    <t>61 to 74</t>
+  </si>
+  <si>
+    <t>arborea</t>
+  </si>
+  <si>
+    <t>canadensis</t>
+  </si>
+  <si>
+    <t>laevis</t>
+  </si>
+  <si>
+    <t>Footnote: In an additional test on excised embryos, germination was 82% (Brinkman 1974).</t>
+  </si>
+  <si>
+    <t>Footnote: In an additional test on excised embryos, germination was 95% (Hilton and others 1965)</t>
+  </si>
+  <si>
+    <t>Crataegus</t>
+  </si>
+  <si>
+    <t>anomala</t>
+  </si>
+  <si>
+    <t>douglasii</t>
+  </si>
+  <si>
+    <t>phaenopyrum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peat or sand </t>
+  </si>
+  <si>
+    <t>crus-galli</t>
+  </si>
+  <si>
+    <t>Soil</t>
+  </si>
+  <si>
+    <t>Germination blotters</t>
+  </si>
+  <si>
+    <t>Peat</t>
+  </si>
+  <si>
+    <t>mollis</t>
+  </si>
+  <si>
+    <t>sanguinea</t>
+  </si>
+  <si>
+    <t>tracyi</t>
+  </si>
+  <si>
+    <t>succulenta</t>
+  </si>
+  <si>
+    <t>punctata</t>
+  </si>
+  <si>
+    <t>42 to 50</t>
+  </si>
+  <si>
+    <t>35 to 40</t>
+  </si>
+  <si>
+    <t>35 to 45</t>
+  </si>
+  <si>
+    <t>8 or fewer</t>
+  </si>
+  <si>
+    <t>2 to 9</t>
+  </si>
+  <si>
+    <t>84 to 112</t>
+  </si>
+  <si>
+    <t>5 to 10</t>
+  </si>
+  <si>
+    <t>110 to 140</t>
+  </si>
+  <si>
+    <t>sulfuric acid</t>
+  </si>
+  <si>
+    <t>Cold and warm strat and pretreatmenttaken from Table 4 but had two rows so I took the treatments easiest to enter (see footnote of Table 5)</t>
+  </si>
+  <si>
+    <t>Cold and warm strat and pretreatmenttaken from Table 4 but had two rows so I took the treatments easiest to enter (see footnote of Table 5); warm strat temp of 21</t>
+  </si>
+  <si>
+    <t>Cold and warm strat and pretreatmenttaken from Table 4 (see footnote of Table 5)</t>
+  </si>
+  <si>
+    <t>Cold and warm strat and pretreatmenttaken from Table 4 but had two rows so I took first row (see footnote of Table 5); warm strat temp of 25</t>
+  </si>
+  <si>
+    <t>Cold and warm strat and pretreatmenttaken from Table 4 (see footnote of Table 5); warm strat temp of 21</t>
+  </si>
+  <si>
+    <t>Cold and warm strat and pretreatmenttaken from Table 4 but had two rows so I took first row (see footnote of Table 5); warm strat temp of 21-25</t>
+  </si>
+  <si>
+    <t>Cold and warm strat and pretreatmenttaken from Table 4 (see footnote of Table 5).</t>
+  </si>
+  <si>
+    <t>Cold and warm strat and pretreatmenttaken from Table 4 (see footnote of Table 5); warm strat temp of 21-27; took averages of days for warm and cold strat and pretreatment</t>
+  </si>
+  <si>
+    <t>Cupressus</t>
+  </si>
+  <si>
+    <t>forbesii</t>
+  </si>
+  <si>
+    <t>bakeri</t>
+  </si>
+  <si>
+    <t>arizonica ssp. nevadensis</t>
+  </si>
+  <si>
+    <t>macnabiana</t>
+  </si>
+  <si>
+    <t>macrocarpa</t>
+  </si>
+  <si>
+    <t>sargentii</t>
+  </si>
+  <si>
+    <t>sempervirens does not have germination data so skipped that line</t>
+  </si>
+  <si>
+    <t>goveniana ssp. pygmaea</t>
+  </si>
+  <si>
+    <t>Table says these are stratified seeds, based on text we could guess that means 30 days at 20 C (but other values are given so this is probably not worth entering)</t>
+  </si>
+  <si>
+    <t>some I suspect (see notes)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -259,6 +477,13 @@
       <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -282,18 +507,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -574,10 +807,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ28"/>
+  <dimension ref="A1:AJ36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -681,7 +914,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.2">
@@ -689,7 +922,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.2">
@@ -697,7 +930,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.2">
@@ -705,7 +938,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.2">
@@ -713,7 +946,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.2">
@@ -721,7 +954,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.2">
@@ -729,7 +962,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.2">
@@ -737,7 +970,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.2">
@@ -745,7 +978,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.2">
@@ -753,7 +986,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -761,31 +994,31 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -793,7 +1026,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -801,7 +1034,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -809,7 +1042,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -825,7 +1058,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -841,7 +1074,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -849,113 +1082,155 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
         <v>53</v>
+      </c>
+      <c r="B30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4AC4DDB-17EE-463A-9304-F699F6DBC2E2}">
-  <dimension ref="A1:AC3"/>
+  <dimension ref="A1:AD29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:29" s="3" customFormat="1" ht="80" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:30" s="5" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Z1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AA1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AB1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="2"/>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AC1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>248</v>
       </c>
@@ -963,19 +1238,19 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="F2" t="s">
-        <v>58</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>62</v>
+        <v>69</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>70</v>
       </c>
       <c r="L2" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="M2">
         <v>16</v>
@@ -992,11 +1267,9 @@
       <c r="U2">
         <v>70</v>
       </c>
-      <c r="V2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="V2" s="7"/>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>248</v>
       </c>
@@ -1004,16 +1277,16 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="F3" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="J3" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="L3">
         <v>120</v>
@@ -1035,6 +1308,990 @@
       </c>
       <c r="V3">
         <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>248</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J4" t="s">
+        <v>70</v>
+      </c>
+      <c r="L4" t="s">
+        <v>77</v>
+      </c>
+      <c r="M4">
+        <v>6</v>
+      </c>
+      <c r="N4">
+        <v>30</v>
+      </c>
+      <c r="O4">
+        <v>20</v>
+      </c>
+      <c r="Q4">
+        <v>31</v>
+      </c>
+      <c r="T4">
+        <v>10</v>
+      </c>
+      <c r="U4">
+        <v>2</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>248</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" t="s">
+        <v>75</v>
+      </c>
+      <c r="J5" t="s">
+        <v>70</v>
+      </c>
+      <c r="L5" t="s">
+        <v>78</v>
+      </c>
+      <c r="M5">
+        <v>16</v>
+      </c>
+      <c r="N5">
+        <v>30</v>
+      </c>
+      <c r="O5">
+        <v>20</v>
+      </c>
+      <c r="T5">
+        <v>54</v>
+      </c>
+      <c r="U5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>248</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" t="s">
+        <v>83</v>
+      </c>
+      <c r="J6" t="s">
+        <v>70</v>
+      </c>
+      <c r="L6">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>248</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7" t="s">
+        <v>76</v>
+      </c>
+      <c r="J7" t="s">
+        <v>70</v>
+      </c>
+      <c r="L7" t="s">
+        <v>79</v>
+      </c>
+      <c r="N7">
+        <v>20</v>
+      </c>
+      <c r="O7">
+        <v>20</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>80</v>
+      </c>
+      <c r="T7" t="s">
+        <v>81</v>
+      </c>
+      <c r="U7">
+        <v>4</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>454</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" t="s">
+        <v>88</v>
+      </c>
+      <c r="F8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G8">
+        <f>4.5*60</f>
+        <v>270</v>
+      </c>
+      <c r="I8" t="s">
+        <v>109</v>
+      </c>
+      <c r="J8" t="s">
+        <v>105</v>
+      </c>
+      <c r="L8">
+        <v>180</v>
+      </c>
+      <c r="M8" t="s">
+        <v>104</v>
+      </c>
+      <c r="N8">
+        <v>8</v>
+      </c>
+      <c r="O8">
+        <v>2</v>
+      </c>
+      <c r="Q8">
+        <v>180</v>
+      </c>
+      <c r="T8">
+        <v>35</v>
+      </c>
+      <c r="U8">
+        <v>1</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>454</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F9" t="s">
+        <v>93</v>
+      </c>
+      <c r="J9">
+        <v>7</v>
+      </c>
+      <c r="K9">
+        <v>120</v>
+      </c>
+      <c r="L9">
+        <v>135</v>
+      </c>
+      <c r="M9" t="s">
+        <v>104</v>
+      </c>
+      <c r="N9">
+        <v>21</v>
+      </c>
+      <c r="O9">
+        <v>21</v>
+      </c>
+      <c r="Q9">
+        <v>21</v>
+      </c>
+      <c r="T9">
+        <v>73</v>
+      </c>
+      <c r="U9">
+        <v>1</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>454</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D10" t="s">
+        <v>89</v>
+      </c>
+      <c r="F10" t="s">
+        <v>91</v>
+      </c>
+      <c r="G10">
+        <f>1.25*60</f>
+        <v>75</v>
+      </c>
+      <c r="I10" t="s">
+        <v>109</v>
+      </c>
+      <c r="J10">
+        <v>5</v>
+      </c>
+      <c r="L10" t="s">
+        <v>106</v>
+      </c>
+      <c r="M10" t="s">
+        <v>104</v>
+      </c>
+      <c r="N10">
+        <v>21</v>
+      </c>
+      <c r="O10">
+        <v>21</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>103</v>
+      </c>
+      <c r="T10">
+        <v>30</v>
+      </c>
+      <c r="U10">
+        <v>6</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>454</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" t="s">
+        <v>96</v>
+      </c>
+      <c r="F11" t="s">
+        <v>93</v>
+      </c>
+      <c r="G11">
+        <v>120</v>
+      </c>
+      <c r="I11" t="s">
+        <v>109</v>
+      </c>
+      <c r="J11">
+        <v>5</v>
+      </c>
+      <c r="K11">
+        <v>90</v>
+      </c>
+      <c r="L11">
+        <v>120</v>
+      </c>
+      <c r="M11" t="s">
+        <v>104</v>
+      </c>
+      <c r="N11">
+        <v>21</v>
+      </c>
+      <c r="O11">
+        <v>21</v>
+      </c>
+      <c r="T11" t="s">
+        <v>101</v>
+      </c>
+      <c r="U11">
+        <v>3</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>454</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F12" t="s">
+        <v>93</v>
+      </c>
+      <c r="J12" t="s">
+        <v>107</v>
+      </c>
+      <c r="L12">
+        <v>135</v>
+      </c>
+      <c r="M12" t="s">
+        <v>104</v>
+      </c>
+      <c r="N12">
+        <v>21</v>
+      </c>
+      <c r="O12">
+        <v>21</v>
+      </c>
+      <c r="T12">
+        <v>71</v>
+      </c>
+      <c r="U12">
+        <v>2</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>454</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" t="s">
+        <v>90</v>
+      </c>
+      <c r="F13" t="s">
+        <v>95</v>
+      </c>
+      <c r="M13" t="s">
+        <v>104</v>
+      </c>
+      <c r="N13">
+        <v>5</v>
+      </c>
+      <c r="O13">
+        <v>5</v>
+      </c>
+      <c r="Q13">
+        <v>135</v>
+      </c>
+      <c r="T13">
+        <v>92</v>
+      </c>
+      <c r="U13">
+        <v>1</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>454</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" t="s">
+        <v>100</v>
+      </c>
+      <c r="F14" t="s">
+        <v>95</v>
+      </c>
+      <c r="J14" t="s">
+        <v>107</v>
+      </c>
+      <c r="K14">
+        <v>120</v>
+      </c>
+      <c r="L14">
+        <v>135</v>
+      </c>
+      <c r="M14" t="s">
+        <v>104</v>
+      </c>
+      <c r="N14" s="8">
+        <v>21</v>
+      </c>
+      <c r="O14" s="8">
+        <v>21</v>
+      </c>
+      <c r="Q14">
+        <v>21</v>
+      </c>
+      <c r="T14">
+        <v>60</v>
+      </c>
+      <c r="U14">
+        <v>1</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>454</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" t="s">
+        <v>97</v>
+      </c>
+      <c r="F15" t="s">
+        <v>95</v>
+      </c>
+      <c r="G15">
+        <v>120</v>
+      </c>
+      <c r="I15" t="s">
+        <v>109</v>
+      </c>
+      <c r="J15">
+        <v>5</v>
+      </c>
+      <c r="K15">
+        <v>21</v>
+      </c>
+      <c r="L15">
+        <v>135</v>
+      </c>
+      <c r="M15" t="s">
+        <v>104</v>
+      </c>
+      <c r="N15" s="8">
+        <v>21</v>
+      </c>
+      <c r="O15" s="8">
+        <v>21</v>
+      </c>
+      <c r="Q15">
+        <v>21</v>
+      </c>
+      <c r="T15">
+        <v>73</v>
+      </c>
+      <c r="U15">
+        <v>1</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>454</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" t="s">
+        <v>97</v>
+      </c>
+      <c r="F16" t="s">
+        <v>95</v>
+      </c>
+      <c r="G16">
+        <v>120</v>
+      </c>
+      <c r="I16" t="s">
+        <v>109</v>
+      </c>
+      <c r="J16">
+        <v>5</v>
+      </c>
+      <c r="K16">
+        <v>21</v>
+      </c>
+      <c r="L16">
+        <v>21</v>
+      </c>
+      <c r="M16" t="s">
+        <v>104</v>
+      </c>
+      <c r="N16">
+        <v>4</v>
+      </c>
+      <c r="O16">
+        <v>7</v>
+      </c>
+      <c r="Q16">
+        <v>30</v>
+      </c>
+      <c r="T16">
+        <v>50</v>
+      </c>
+      <c r="U16">
+        <v>2</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>454</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" t="s">
+        <v>99</v>
+      </c>
+      <c r="F17" t="s">
+        <v>93</v>
+      </c>
+      <c r="G17">
+        <v>30</v>
+      </c>
+      <c r="I17" t="s">
+        <v>109</v>
+      </c>
+      <c r="J17">
+        <v>4</v>
+      </c>
+      <c r="L17" t="s">
+        <v>108</v>
+      </c>
+      <c r="M17" t="s">
+        <v>104</v>
+      </c>
+      <c r="T17" t="s">
+        <v>102</v>
+      </c>
+      <c r="U17">
+        <v>2</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>454</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18" t="s">
+        <v>98</v>
+      </c>
+      <c r="F18" t="s">
+        <v>94</v>
+      </c>
+      <c r="G18">
+        <f>(AVERAGE(0,0.5,2.5,4.5))*60</f>
+        <v>112.5</v>
+      </c>
+      <c r="I18" t="s">
+        <v>109</v>
+      </c>
+      <c r="J18">
+        <v>4</v>
+      </c>
+      <c r="K18">
+        <f>200/4</f>
+        <v>50</v>
+      </c>
+      <c r="L18">
+        <f>120/3</f>
+        <v>40</v>
+      </c>
+      <c r="M18">
+        <v>16</v>
+      </c>
+      <c r="N18">
+        <v>16</v>
+      </c>
+      <c r="O18">
+        <v>16</v>
+      </c>
+      <c r="Q18">
+        <v>28</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <v>2</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>464</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>118</v>
+      </c>
+      <c r="D19" t="s">
+        <v>121</v>
+      </c>
+      <c r="K19" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q19">
+        <v>20</v>
+      </c>
+      <c r="T19">
+        <v>26</v>
+      </c>
+      <c r="U19">
+        <v>9</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>464</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>118</v>
+      </c>
+      <c r="D20" t="s">
+        <v>121</v>
+      </c>
+      <c r="K20" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q20">
+        <v>6</v>
+      </c>
+      <c r="T20">
+        <v>6</v>
+      </c>
+      <c r="U20">
+        <v>1</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>464</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>118</v>
+      </c>
+      <c r="D21" t="s">
+        <v>120</v>
+      </c>
+      <c r="K21" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q21">
+        <v>30</v>
+      </c>
+      <c r="T21">
+        <v>12</v>
+      </c>
+      <c r="U21">
+        <v>2</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>464</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>118</v>
+      </c>
+      <c r="D22" t="s">
+        <v>119</v>
+      </c>
+      <c r="K22" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q22">
+        <v>30</v>
+      </c>
+      <c r="T22">
+        <v>12</v>
+      </c>
+      <c r="U22">
+        <v>2</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>464</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>118</v>
+      </c>
+      <c r="D23" t="s">
+        <v>126</v>
+      </c>
+      <c r="K23" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q23">
+        <v>30</v>
+      </c>
+      <c r="T23">
+        <v>22</v>
+      </c>
+      <c r="U23">
+        <v>2</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>464</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>118</v>
+      </c>
+      <c r="D24" t="s">
+        <v>126</v>
+      </c>
+      <c r="K24" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q24">
+        <v>30</v>
+      </c>
+      <c r="T24">
+        <v>31</v>
+      </c>
+      <c r="U24">
+        <v>2</v>
+      </c>
+      <c r="AD24" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>464</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>118</v>
+      </c>
+      <c r="D25" t="s">
+        <v>122</v>
+      </c>
+      <c r="K25" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q25">
+        <v>30</v>
+      </c>
+      <c r="T25">
+        <v>1</v>
+      </c>
+      <c r="U25">
+        <v>1</v>
+      </c>
+      <c r="AD25" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>464</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
+        <v>118</v>
+      </c>
+      <c r="D26" t="s">
+        <v>122</v>
+      </c>
+      <c r="K26" t="s">
+        <v>128</v>
+      </c>
+      <c r="U26">
+        <v>15</v>
+      </c>
+      <c r="AD26" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>464</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27" t="s">
+        <v>118</v>
+      </c>
+      <c r="D27" t="s">
+        <v>123</v>
+      </c>
+      <c r="K27" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q27">
+        <v>30</v>
+      </c>
+      <c r="T27">
+        <v>24</v>
+      </c>
+      <c r="U27">
+        <v>4</v>
+      </c>
+      <c r="AD27" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>464</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28" t="s">
+        <v>118</v>
+      </c>
+      <c r="D28" t="s">
+        <v>123</v>
+      </c>
+      <c r="K28" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q28">
+        <v>30</v>
+      </c>
+      <c r="T28">
+        <v>14</v>
+      </c>
+      <c r="U28">
+        <v>37</v>
+      </c>
+      <c r="AD28" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>464</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="C29" t="s">
+        <v>118</v>
+      </c>
+      <c r="D29" t="s">
+        <v>124</v>
+      </c>
+      <c r="K29" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q29">
+        <v>30</v>
+      </c>
+      <c r="T29">
+        <v>13</v>
+      </c>
+      <c r="U29">
+        <v>2</v>
+      </c>
+      <c r="AD29" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated to new file my USDA data entry
</commit_message>
<xml_diff>
--- a/analyses/scrapeUSDAseedmanual/scraping/usdaDataScraping_EMW.xlsx
+++ b/analyses/scrapeUSDAseedmanual/scraping/usdaDataScraping_EMW.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lizzie/Documents/git/projects/egret/analyses/scrapeUSDAseedmanual/scraping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB27D429-5413-4C49-AC5D-39E1FD42A8FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1FD80B-4D3A-6F4F-95CB-76C37A844E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22400" yWindow="500" windowWidth="24780" windowHeight="23620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1820" yWindow="760" windowWidth="27740" windowHeight="14520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meta" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="133">
   <si>
     <t>pdf_page_number</t>
   </si>
@@ -65,9 +65,6 @@
     <t>pretreatment</t>
   </si>
   <si>
-    <t>stratification_temp_C</t>
-  </si>
-  <si>
     <t>warm_stratification_days</t>
   </si>
   <si>
@@ -152,10 +149,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>temperature of stratification</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>warm stratification duration</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -274,6 +267,22 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>cold_stratification_temp_C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>warm_stratification_temp_C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>temperature of warm stratification</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>temperature of cold stratification</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Amelanchier</t>
   </si>
   <si>
@@ -283,27 +292,111 @@
     <t>sand</t>
   </si>
   <si>
+    <t>sand or blotters</t>
+  </si>
+  <si>
+    <t>alnifolia var. semiintegrifolia</t>
+  </si>
+  <si>
+    <t>kimpack</t>
+  </si>
+  <si>
+    <t>arborea</t>
+  </si>
+  <si>
+    <t>sand or sand and peat</t>
+  </si>
+  <si>
+    <t>canadensis</t>
+  </si>
+  <si>
+    <t>laevis</t>
+  </si>
+  <si>
+    <t>filter paper</t>
+  </si>
+  <si>
+    <t>Crataegus</t>
+  </si>
+  <si>
+    <t>anomala</t>
+  </si>
+  <si>
+    <t>Soil</t>
+  </si>
+  <si>
+    <t>sulfuric acid</t>
+  </si>
+  <si>
+    <t>crus-galli</t>
+  </si>
+  <si>
+    <t>douglasii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peat or sand </t>
+  </si>
+  <si>
+    <t>mollis</t>
+  </si>
+  <si>
+    <t>phaenopyrum</t>
+  </si>
+  <si>
+    <t>Peat</t>
+  </si>
+  <si>
+    <t>punctata</t>
+  </si>
+  <si>
+    <t>sanguinea</t>
+  </si>
+  <si>
+    <t>succulenta</t>
+  </si>
+  <si>
+    <t>tracyi</t>
+  </si>
+  <si>
+    <t>Germination blotters</t>
+  </si>
+  <si>
+    <t>Cupressus</t>
+  </si>
+  <si>
+    <t>arizonica ssp. nevadensis</t>
+  </si>
+  <si>
+    <t>bakeri</t>
+  </si>
+  <si>
+    <t>forbesii</t>
+  </si>
+  <si>
+    <t>goveniana ssp. pygmaea</t>
+  </si>
+  <si>
+    <t>macnabiana</t>
+  </si>
+  <si>
+    <t>macrocarpa</t>
+  </si>
+  <si>
+    <t>sargentii</t>
+  </si>
+  <si>
     <t>1 to 6</t>
   </si>
   <si>
-    <t>sand or blotters</t>
+    <t>2 to 9</t>
+  </si>
+  <si>
+    <t>5 to 10</t>
   </si>
   <si>
     <t>180+</t>
   </si>
   <si>
-    <t>alnifolia var. semiintegrifolia</t>
-  </si>
-  <si>
-    <t>kimpack</t>
-  </si>
-  <si>
-    <t>sand or sand and peat</t>
-  </si>
-  <si>
-    <t>filter paper</t>
-  </si>
-  <si>
     <t>30 to 90</t>
   </si>
   <si>
@@ -319,13 +412,25 @@
     <t>61 to 74</t>
   </si>
   <si>
-    <t>arborea</t>
-  </si>
-  <si>
-    <t>canadensis</t>
-  </si>
-  <si>
-    <t>laevis</t>
+    <t>8 or fewer</t>
+  </si>
+  <si>
+    <t>84 to 112</t>
+  </si>
+  <si>
+    <t>35 to 45</t>
+  </si>
+  <si>
+    <t>42 to 50</t>
+  </si>
+  <si>
+    <t>110 to 140</t>
+  </si>
+  <si>
+    <t>35 to 40</t>
+  </si>
+  <si>
+    <t>some I suspect (see notes)</t>
   </si>
   <si>
     <t>Footnote: In an additional test on excised embryos, germination was 82% (Brinkman 1974).</t>
@@ -334,75 +439,6 @@
     <t>Footnote: In an additional test on excised embryos, germination was 95% (Hilton and others 1965)</t>
   </si>
   <si>
-    <t>Crataegus</t>
-  </si>
-  <si>
-    <t>anomala</t>
-  </si>
-  <si>
-    <t>douglasii</t>
-  </si>
-  <si>
-    <t>phaenopyrum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Peat or sand </t>
-  </si>
-  <si>
-    <t>crus-galli</t>
-  </si>
-  <si>
-    <t>Soil</t>
-  </si>
-  <si>
-    <t>Germination blotters</t>
-  </si>
-  <si>
-    <t>Peat</t>
-  </si>
-  <si>
-    <t>mollis</t>
-  </si>
-  <si>
-    <t>sanguinea</t>
-  </si>
-  <si>
-    <t>tracyi</t>
-  </si>
-  <si>
-    <t>succulenta</t>
-  </si>
-  <si>
-    <t>punctata</t>
-  </si>
-  <si>
-    <t>42 to 50</t>
-  </si>
-  <si>
-    <t>35 to 40</t>
-  </si>
-  <si>
-    <t>35 to 45</t>
-  </si>
-  <si>
-    <t>8 or fewer</t>
-  </si>
-  <si>
-    <t>2 to 9</t>
-  </si>
-  <si>
-    <t>84 to 112</t>
-  </si>
-  <si>
-    <t>5 to 10</t>
-  </si>
-  <si>
-    <t>110 to 140</t>
-  </si>
-  <si>
-    <t>sulfuric acid</t>
-  </si>
-  <si>
     <t>Cold and warm strat and pretreatmenttaken from Table 4 but had two rows so I took the treatments easiest to enter (see footnote of Table 5)</t>
   </si>
   <si>
@@ -427,37 +463,16 @@
     <t>Cold and warm strat and pretreatmenttaken from Table 4 (see footnote of Table 5); warm strat temp of 21-27; took averages of days for warm and cold strat and pretreatment</t>
   </si>
   <si>
-    <t>Cupressus</t>
-  </si>
-  <si>
-    <t>forbesii</t>
-  </si>
-  <si>
-    <t>bakeri</t>
-  </si>
-  <si>
-    <t>arizonica ssp. nevadensis</t>
-  </si>
-  <si>
-    <t>macnabiana</t>
-  </si>
-  <si>
-    <t>macrocarpa</t>
-  </si>
-  <si>
-    <t>sargentii</t>
+    <t>Table says these are stratified seeds, based on text we could guess that means 30 days at 20 C (but other values are given so this is probably not worth entering)</t>
   </si>
   <si>
     <t>sempervirens does not have germination data so skipped that line</t>
   </si>
   <si>
-    <t>goveniana ssp. pygmaea</t>
-  </si>
-  <si>
-    <t>Table says these are stratified seeds, based on text we could guess that means 30 days at 20 C (but other values are given so this is probably not worth entering)</t>
-  </si>
-  <si>
-    <t>some I suspect (see notes)</t>
+    <t>21 to 25</t>
+  </si>
+  <si>
+    <t>21 to 27</t>
   </si>
 </sst>
 </file>
@@ -807,10 +822,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ36"/>
+  <dimension ref="A1:AJ37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -832,7 +847,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -874,7 +889,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.2">
@@ -882,7 +897,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.2">
@@ -890,7 +905,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.2">
@@ -898,7 +913,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.2">
@@ -906,7 +921,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.2">
@@ -914,7 +929,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.2">
@@ -922,7 +937,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.2">
@@ -930,195 +945,203 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>65</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>52</v>
+      <c r="A29" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>53</v>
+      <c r="A30" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>60</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>63</v>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1130,15 +1153,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4AC4DDB-17EE-463A-9304-F699F6DBC2E2}">
-  <dimension ref="A1:AD29"/>
+  <dimension ref="A1:AE29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:XFD29"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:30" s="5" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" s="5" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1167,70 +1190,73 @@
         <v>8</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="AD1" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AD1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>248</v>
       </c>
@@ -1238,38 +1264,38 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F2" t="s">
-        <v>69</v>
-      </c>
-      <c r="J2" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="M2" t="s">
+        <v>106</v>
+      </c>
+      <c r="N2">
+        <v>16</v>
+      </c>
+      <c r="O2">
+        <v>30</v>
+      </c>
+      <c r="P2">
+        <v>20</v>
+      </c>
+      <c r="R2">
+        <v>30</v>
+      </c>
+      <c r="V2">
         <v>70</v>
       </c>
-      <c r="L2" t="s">
-        <v>72</v>
-      </c>
-      <c r="M2">
-        <v>16</v>
-      </c>
-      <c r="N2">
-        <v>30</v>
-      </c>
-      <c r="O2">
-        <v>20</v>
-      </c>
-      <c r="Q2">
-        <v>30</v>
-      </c>
-      <c r="U2">
-        <v>70</v>
-      </c>
-      <c r="V2" s="7"/>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="W2" s="7"/>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>248</v>
       </c>
@@ -1277,40 +1303,40 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F3" t="s">
-        <v>71</v>
-      </c>
-      <c r="J3" t="s">
-        <v>70</v>
-      </c>
-      <c r="L3">
+        <v>72</v>
+      </c>
+      <c r="L3" t="s">
+        <v>103</v>
+      </c>
+      <c r="M3">
         <v>120</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>0</v>
-      </c>
-      <c r="N3">
-        <v>21</v>
       </c>
       <c r="O3">
         <v>21</v>
       </c>
-      <c r="Q3">
+      <c r="P3">
+        <v>21</v>
+      </c>
+      <c r="R3">
         <v>70</v>
       </c>
-      <c r="U3">
+      <c r="V3">
         <v>62</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>248</v>
       </c>
@@ -1318,7 +1344,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D4" t="s">
         <v>73</v>
@@ -1326,35 +1352,35 @@
       <c r="F4" t="s">
         <v>74</v>
       </c>
-      <c r="J4" t="s">
-        <v>70</v>
-      </c>
       <c r="L4" t="s">
-        <v>77</v>
-      </c>
-      <c r="M4">
+        <v>103</v>
+      </c>
+      <c r="M4" t="s">
+        <v>107</v>
+      </c>
+      <c r="N4">
         <v>6</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>30</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>20</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>31</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>10</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <v>2</v>
       </c>
-      <c r="AD4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>248</v>
       </c>
@@ -1362,37 +1388,37 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D5" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F5" t="s">
-        <v>75</v>
-      </c>
-      <c r="J5" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="L5" t="s">
-        <v>78</v>
-      </c>
-      <c r="M5">
+        <v>103</v>
+      </c>
+      <c r="M5" t="s">
+        <v>108</v>
+      </c>
+      <c r="N5">
         <v>16</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>30</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>20</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>54</v>
       </c>
-      <c r="U5">
+      <c r="V5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>248</v>
       </c>
@@ -1400,19 +1426,19 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D6" t="s">
-        <v>83</v>
-      </c>
-      <c r="J6" t="s">
-        <v>70</v>
-      </c>
-      <c r="L6">
+        <v>77</v>
+      </c>
+      <c r="L6" t="s">
+        <v>103</v>
+      </c>
+      <c r="M6">
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>248</v>
       </c>
@@ -1420,40 +1446,40 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D7" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="F7" t="s">
-        <v>76</v>
-      </c>
-      <c r="J7" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="L7" t="s">
-        <v>79</v>
-      </c>
-      <c r="N7">
-        <v>20</v>
+        <v>103</v>
+      </c>
+      <c r="M7" t="s">
+        <v>109</v>
       </c>
       <c r="O7">
         <v>20</v>
       </c>
-      <c r="Q7" t="s">
-        <v>80</v>
-      </c>
-      <c r="T7" t="s">
-        <v>81</v>
-      </c>
-      <c r="U7">
+      <c r="P7">
+        <v>20</v>
+      </c>
+      <c r="R7" t="s">
+        <v>110</v>
+      </c>
+      <c r="U7" t="s">
+        <v>111</v>
+      </c>
+      <c r="V7">
         <v>4</v>
       </c>
-      <c r="AD7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>454</v>
       </c>
@@ -1461,50 +1487,50 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D8" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="F8" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="G8">
         <f>4.5*60</f>
         <v>270</v>
       </c>
       <c r="I8" t="s">
-        <v>109</v>
-      </c>
-      <c r="J8" t="s">
-        <v>105</v>
-      </c>
-      <c r="L8">
+        <v>83</v>
+      </c>
+      <c r="L8" t="s">
+        <v>104</v>
+      </c>
+      <c r="M8">
         <v>180</v>
       </c>
-      <c r="M8" t="s">
-        <v>104</v>
-      </c>
-      <c r="N8">
+      <c r="N8" t="s">
+        <v>112</v>
+      </c>
+      <c r="O8">
         <v>8</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>2</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>180</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <v>35</v>
       </c>
-      <c r="U8">
+      <c r="V8">
         <v>1</v>
       </c>
-      <c r="AD8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>454</v>
       </c>
@@ -1512,46 +1538,49 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D9" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="F9" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="J9">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="K9">
         <v>120</v>
       </c>
       <c r="L9">
+        <v>7</v>
+      </c>
+      <c r="M9">
         <v>135</v>
       </c>
-      <c r="M9" t="s">
-        <v>104</v>
-      </c>
-      <c r="N9">
-        <v>21</v>
+      <c r="N9" t="s">
+        <v>112</v>
       </c>
       <c r="O9">
         <v>21</v>
       </c>
-      <c r="Q9">
+      <c r="P9">
         <v>21</v>
       </c>
-      <c r="T9">
+      <c r="R9">
+        <v>21</v>
+      </c>
+      <c r="U9">
         <v>73</v>
       </c>
-      <c r="U9">
+      <c r="V9">
         <v>1</v>
       </c>
-      <c r="AD9" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>454</v>
       </c>
@@ -1559,50 +1588,50 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D10" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F10" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="G10">
         <f>1.25*60</f>
         <v>75</v>
       </c>
       <c r="I10" t="s">
-        <v>109</v>
-      </c>
-      <c r="J10">
-        <v>5</v>
-      </c>
-      <c r="L10" t="s">
-        <v>106</v>
+        <v>83</v>
+      </c>
+      <c r="L10">
+        <v>5</v>
       </c>
       <c r="M10" t="s">
-        <v>104</v>
-      </c>
-      <c r="N10">
-        <v>21</v>
+        <v>113</v>
+      </c>
+      <c r="N10" t="s">
+        <v>112</v>
       </c>
       <c r="O10">
         <v>21</v>
       </c>
-      <c r="Q10" t="s">
-        <v>103</v>
-      </c>
-      <c r="T10">
+      <c r="P10">
+        <v>21</v>
+      </c>
+      <c r="R10" t="s">
+        <v>114</v>
+      </c>
+      <c r="U10">
         <v>30</v>
       </c>
-      <c r="U10">
+      <c r="V10">
         <v>6</v>
       </c>
-      <c r="AD10" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>454</v>
       </c>
@@ -1610,49 +1639,52 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" t="s">
         <v>87</v>
       </c>
-      <c r="D11" t="s">
-        <v>96</v>
-      </c>
       <c r="F11" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="G11">
         <v>120</v>
       </c>
       <c r="I11" t="s">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="J11">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="K11">
         <v>90</v>
       </c>
       <c r="L11">
+        <v>5</v>
+      </c>
+      <c r="M11">
         <v>120</v>
       </c>
-      <c r="M11" t="s">
-        <v>104</v>
-      </c>
-      <c r="N11">
-        <v>21</v>
+      <c r="N11" t="s">
+        <v>112</v>
       </c>
       <c r="O11">
         <v>21</v>
       </c>
-      <c r="T11" t="s">
-        <v>101</v>
-      </c>
-      <c r="U11">
+      <c r="P11">
+        <v>21</v>
+      </c>
+      <c r="U11" t="s">
+        <v>115</v>
+      </c>
+      <c r="V11">
         <v>3</v>
       </c>
-      <c r="AD11" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>454</v>
       </c>
@@ -1660,40 +1692,40 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F12" t="s">
-        <v>93</v>
-      </c>
-      <c r="J12" t="s">
-        <v>107</v>
-      </c>
-      <c r="L12">
+        <v>82</v>
+      </c>
+      <c r="L12" t="s">
+        <v>105</v>
+      </c>
+      <c r="M12">
         <v>135</v>
       </c>
-      <c r="M12" t="s">
-        <v>104</v>
-      </c>
-      <c r="N12">
-        <v>21</v>
+      <c r="N12" t="s">
+        <v>112</v>
       </c>
       <c r="O12">
         <v>21</v>
       </c>
-      <c r="T12">
+      <c r="P12">
+        <v>21</v>
+      </c>
+      <c r="U12">
         <v>71</v>
       </c>
-      <c r="U12">
+      <c r="V12">
         <v>2</v>
       </c>
-      <c r="AD12" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>454</v>
       </c>
@@ -1701,37 +1733,37 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F13" t="s">
-        <v>95</v>
-      </c>
-      <c r="M13" t="s">
-        <v>104</v>
-      </c>
-      <c r="N13">
-        <v>5</v>
+        <v>89</v>
+      </c>
+      <c r="N13" t="s">
+        <v>112</v>
       </c>
       <c r="O13">
         <v>5</v>
       </c>
-      <c r="Q13">
+      <c r="P13">
+        <v>5</v>
+      </c>
+      <c r="R13">
         <v>135</v>
       </c>
-      <c r="T13">
+      <c r="U13">
         <v>92</v>
       </c>
-      <c r="U13">
+      <c r="V13">
         <v>1</v>
       </c>
-      <c r="AD13" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE13" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>454</v>
       </c>
@@ -1739,46 +1771,46 @@
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D14" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="F14" t="s">
-        <v>95</v>
-      </c>
-      <c r="J14" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="K14">
         <v>120</v>
       </c>
-      <c r="L14">
+      <c r="L14" t="s">
+        <v>105</v>
+      </c>
+      <c r="M14">
         <v>135</v>
       </c>
-      <c r="M14" t="s">
-        <v>104</v>
-      </c>
-      <c r="N14" s="8">
-        <v>21</v>
+      <c r="N14" t="s">
+        <v>112</v>
       </c>
       <c r="O14" s="8">
         <v>21</v>
       </c>
-      <c r="Q14">
+      <c r="P14" s="8">
         <v>21</v>
       </c>
-      <c r="T14">
+      <c r="R14">
+        <v>21</v>
+      </c>
+      <c r="U14">
         <v>60</v>
       </c>
-      <c r="U14">
+      <c r="V14">
         <v>1</v>
       </c>
-      <c r="AD14" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>454</v>
       </c>
@@ -1786,52 +1818,55 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D15" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="F15" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="G15">
         <v>120</v>
       </c>
       <c r="I15" t="s">
-        <v>109</v>
-      </c>
-      <c r="J15">
-        <v>5</v>
+        <v>83</v>
+      </c>
+      <c r="J15" t="s">
+        <v>131</v>
       </c>
       <c r="K15">
         <v>21</v>
       </c>
       <c r="L15">
+        <v>5</v>
+      </c>
+      <c r="M15">
         <v>135</v>
       </c>
-      <c r="M15" t="s">
-        <v>104</v>
-      </c>
-      <c r="N15" s="8">
-        <v>21</v>
+      <c r="N15" t="s">
+        <v>112</v>
       </c>
       <c r="O15" s="8">
         <v>21</v>
       </c>
-      <c r="Q15">
+      <c r="P15" s="8">
         <v>21</v>
       </c>
-      <c r="T15">
+      <c r="R15">
+        <v>21</v>
+      </c>
+      <c r="U15">
         <v>73</v>
       </c>
-      <c r="U15">
+      <c r="V15">
         <v>1</v>
       </c>
-      <c r="AD15" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE15" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>454</v>
       </c>
@@ -1839,52 +1874,55 @@
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D16" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="F16" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="G16">
         <v>120</v>
       </c>
       <c r="I16" t="s">
-        <v>109</v>
-      </c>
-      <c r="J16">
-        <v>5</v>
+        <v>83</v>
+      </c>
+      <c r="J16" t="s">
+        <v>131</v>
       </c>
       <c r="K16">
         <v>21</v>
       </c>
       <c r="L16">
+        <v>5</v>
+      </c>
+      <c r="M16">
         <v>21</v>
       </c>
-      <c r="M16" t="s">
-        <v>104</v>
-      </c>
-      <c r="N16">
+      <c r="N16" t="s">
+        <v>112</v>
+      </c>
+      <c r="O16">
         <v>4</v>
       </c>
-      <c r="O16">
+      <c r="P16">
         <v>7</v>
       </c>
-      <c r="Q16">
+      <c r="R16">
         <v>30</v>
       </c>
-      <c r="T16">
+      <c r="U16">
         <v>50</v>
       </c>
-      <c r="U16">
+      <c r="V16">
         <v>2</v>
       </c>
-      <c r="AD16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>454</v>
       </c>
@@ -1892,40 +1930,40 @@
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D17" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="F17" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="G17">
         <v>30</v>
       </c>
       <c r="I17" t="s">
-        <v>109</v>
-      </c>
-      <c r="J17">
+        <v>83</v>
+      </c>
+      <c r="L17">
         <v>4</v>
       </c>
-      <c r="L17" t="s">
-        <v>108</v>
-      </c>
       <c r="M17" t="s">
-        <v>104</v>
-      </c>
-      <c r="T17" t="s">
-        <v>102</v>
-      </c>
-      <c r="U17">
+        <v>116</v>
+      </c>
+      <c r="N17" t="s">
+        <v>112</v>
+      </c>
+      <c r="U17" t="s">
+        <v>117</v>
+      </c>
+      <c r="V17">
         <v>2</v>
       </c>
-      <c r="AD17" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE17" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>454</v>
       </c>
@@ -1933,10 +1971,10 @@
         <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D18" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F18" t="s">
         <v>94</v>
@@ -1946,42 +1984,45 @@
         <v>112.5</v>
       </c>
       <c r="I18" t="s">
-        <v>109</v>
-      </c>
-      <c r="J18">
-        <v>4</v>
+        <v>83</v>
+      </c>
+      <c r="J18" t="s">
+        <v>132</v>
       </c>
       <c r="K18">
         <f>200/4</f>
         <v>50</v>
       </c>
       <c r="L18">
+        <v>4</v>
+      </c>
+      <c r="M18">
         <f>120/3</f>
         <v>40</v>
       </c>
-      <c r="M18">
-        <v>16</v>
-      </c>
       <c r="N18">
         <v>16</v>
       </c>
       <c r="O18">
         <v>16</v>
       </c>
-      <c r="Q18">
+      <c r="P18">
+        <v>16</v>
+      </c>
+      <c r="R18">
         <v>28</v>
       </c>
-      <c r="T18">
+      <c r="U18">
         <v>0</v>
       </c>
-      <c r="U18">
+      <c r="V18">
         <v>2</v>
       </c>
-      <c r="AD18" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE18" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>464</v>
       </c>
@@ -1989,28 +2030,28 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
+        <v>95</v>
+      </c>
+      <c r="D19" t="s">
+        <v>96</v>
+      </c>
+      <c r="K19" t="s">
         <v>118</v>
       </c>
-      <c r="D19" t="s">
-        <v>121</v>
-      </c>
-      <c r="K19" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q19">
+      <c r="R19">
         <v>20</v>
       </c>
-      <c r="T19">
+      <c r="U19">
         <v>26</v>
       </c>
-      <c r="U19">
+      <c r="V19">
         <v>9</v>
       </c>
-      <c r="AD19" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>464</v>
       </c>
@@ -2018,28 +2059,28 @@
         <v>4</v>
       </c>
       <c r="C20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D20" t="s">
+        <v>96</v>
+      </c>
+      <c r="K20" t="s">
         <v>118</v>
       </c>
-      <c r="D20" t="s">
-        <v>121</v>
-      </c>
-      <c r="K20" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q20">
+      <c r="R20">
         <v>6</v>
       </c>
-      <c r="T20">
+      <c r="U20">
         <v>6</v>
       </c>
-      <c r="U20">
+      <c r="V20">
         <v>1</v>
       </c>
-      <c r="AD20" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE20" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>464</v>
       </c>
@@ -2047,28 +2088,28 @@
         <v>4</v>
       </c>
       <c r="C21" t="s">
+        <v>95</v>
+      </c>
+      <c r="D21" t="s">
+        <v>97</v>
+      </c>
+      <c r="K21" t="s">
         <v>118</v>
       </c>
-      <c r="D21" t="s">
-        <v>120</v>
-      </c>
-      <c r="K21" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q21">
+      <c r="R21">
         <v>30</v>
       </c>
-      <c r="T21">
+      <c r="U21">
         <v>12</v>
       </c>
-      <c r="U21">
+      <c r="V21">
         <v>2</v>
       </c>
-      <c r="AD21" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>464</v>
       </c>
@@ -2076,28 +2117,28 @@
         <v>4</v>
       </c>
       <c r="C22" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K22" t="s">
         <v>118</v>
       </c>
-      <c r="D22" t="s">
-        <v>119</v>
-      </c>
-      <c r="K22" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q22">
+      <c r="R22">
         <v>30</v>
       </c>
-      <c r="T22">
+      <c r="U22">
         <v>12</v>
       </c>
-      <c r="U22">
+      <c r="V22">
         <v>2</v>
       </c>
-      <c r="AD22" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>464</v>
       </c>
@@ -2105,28 +2146,28 @@
         <v>4</v>
       </c>
       <c r="C23" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" t="s">
+        <v>99</v>
+      </c>
+      <c r="K23" t="s">
         <v>118</v>
       </c>
-      <c r="D23" t="s">
-        <v>126</v>
-      </c>
-      <c r="K23" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q23">
+      <c r="R23">
         <v>30</v>
       </c>
-      <c r="T23">
+      <c r="U23">
         <v>22</v>
       </c>
-      <c r="U23">
+      <c r="V23">
         <v>2</v>
       </c>
-      <c r="AD23" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE23" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>464</v>
       </c>
@@ -2134,28 +2175,28 @@
         <v>4</v>
       </c>
       <c r="C24" t="s">
+        <v>95</v>
+      </c>
+      <c r="D24" t="s">
+        <v>99</v>
+      </c>
+      <c r="K24" t="s">
         <v>118</v>
       </c>
-      <c r="D24" t="s">
-        <v>126</v>
-      </c>
-      <c r="K24" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q24">
+      <c r="R24">
         <v>30</v>
       </c>
-      <c r="T24">
+      <c r="U24">
         <v>31</v>
       </c>
-      <c r="U24">
+      <c r="V24">
         <v>2</v>
       </c>
-      <c r="AD24" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE24" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>464</v>
       </c>
@@ -2163,28 +2204,28 @@
         <v>4</v>
       </c>
       <c r="C25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D25" t="s">
+        <v>100</v>
+      </c>
+      <c r="K25" t="s">
         <v>118</v>
       </c>
-      <c r="D25" t="s">
-        <v>122</v>
-      </c>
-      <c r="K25" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q25">
+      <c r="R25">
         <v>30</v>
-      </c>
-      <c r="T25">
-        <v>1</v>
       </c>
       <c r="U25">
         <v>1</v>
       </c>
-      <c r="AD25" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="V25">
+        <v>1</v>
+      </c>
+      <c r="AE25" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>464</v>
       </c>
@@ -2192,22 +2233,22 @@
         <v>4</v>
       </c>
       <c r="C26" t="s">
+        <v>95</v>
+      </c>
+      <c r="D26" t="s">
+        <v>100</v>
+      </c>
+      <c r="K26" t="s">
         <v>118</v>
       </c>
-      <c r="D26" t="s">
-        <v>122</v>
-      </c>
-      <c r="K26" t="s">
-        <v>128</v>
-      </c>
-      <c r="U26">
+      <c r="V26">
         <v>15</v>
       </c>
-      <c r="AD26" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE26" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>464</v>
       </c>
@@ -2215,28 +2256,28 @@
         <v>4</v>
       </c>
       <c r="C27" t="s">
+        <v>95</v>
+      </c>
+      <c r="D27" t="s">
+        <v>101</v>
+      </c>
+      <c r="K27" t="s">
         <v>118</v>
       </c>
-      <c r="D27" t="s">
-        <v>123</v>
-      </c>
-      <c r="K27" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q27">
+      <c r="R27">
         <v>30</v>
       </c>
-      <c r="T27">
+      <c r="U27">
         <v>24</v>
       </c>
-      <c r="U27">
+      <c r="V27">
         <v>4</v>
       </c>
-      <c r="AD27" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE27" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>464</v>
       </c>
@@ -2244,28 +2285,28 @@
         <v>4</v>
       </c>
       <c r="C28" t="s">
+        <v>95</v>
+      </c>
+      <c r="D28" t="s">
+        <v>101</v>
+      </c>
+      <c r="K28" t="s">
         <v>118</v>
       </c>
-      <c r="D28" t="s">
-        <v>123</v>
-      </c>
-      <c r="K28" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q28">
+      <c r="R28">
         <v>30</v>
       </c>
-      <c r="T28">
+      <c r="U28">
         <v>14</v>
       </c>
-      <c r="U28">
+      <c r="V28">
         <v>37</v>
       </c>
-      <c r="AD28" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE28" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>464</v>
       </c>
@@ -2273,25 +2314,25 @@
         <v>4</v>
       </c>
       <c r="C29" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" t="s">
+        <v>102</v>
+      </c>
+      <c r="K29" t="s">
         <v>118</v>
       </c>
-      <c r="D29" t="s">
-        <v>124</v>
-      </c>
-      <c r="K29" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q29">
+      <c r="R29">
         <v>30</v>
       </c>
-      <c r="T29">
+      <c r="U29">
         <v>13</v>
       </c>
-      <c r="U29">
+      <c r="V29">
         <v>2</v>
       </c>
-      <c r="AD29" t="s">
-        <v>125</v>
+      <c r="AE29" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>